<commit_message>
Updated PV Default Costs Spreadsheet
</commit_message>
<xml_diff>
--- a/References/PV Default Costs.xlsx
+++ b/References/PV Default Costs.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="20370" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Proposed 2016.3.14" sheetId="1" r:id="rId1"/>
+    <sheet name="2014.11.24" sheetId="2" r:id="rId2"/>
+    <sheet name="2014.1.14" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>Direct Capital Costs</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>To be included in SAM Version 2016.3.14</t>
+  </si>
+  <si>
+    <t>SAM Version 2014.1.14</t>
+  </si>
+  <si>
+    <t>SAM Version 2014.11.24</t>
   </si>
 </sst>
 </file>
@@ -170,7 +176,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -190,6 +196,15 @@
     <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -505,7 +520,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,18 +535,18 @@
       <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="19"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -788,24 +803,477 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.70498109471139347</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0.71</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.33219565217391261</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0.21</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="16">
+        <f>0.606727822987794+0.21</f>
+        <v>0.81672782298779401</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0.56579275109464489</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="16">
+        <v>0.9469103998436198</v>
+      </c>
+      <c r="C7" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="18">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="16">
+        <v>9.7136303302560914E-2</v>
+      </c>
+      <c r="C10" s="15">
+        <v>5.7294635612556974E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0.81863629229227208</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="14">
+        <f t="shared" ref="B17:D17" si="0">SUM(B3:B7)*(1+B8)*(1+B15*B16)+SUM(B10:B14)</f>
+        <v>3.2878749071410653</v>
+      </c>
+      <c r="C17" s="14">
+        <f t="shared" si="0"/>
+        <v>2.5407422133038966</v>
+      </c>
+      <c r="D17" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9024999999999999</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="10">
+        <v>1</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="14">
+        <f>SUM(B3:B7)*(1+B8)*(1+B15*B16)+SUM(B10:B14)</f>
+        <v>3.7649999999999997</v>
+      </c>
+      <c r="C17" s="14">
+        <f t="shared" ref="C17:D17" si="0">SUM(C3:C7)*(1+C8)*(1+C15*C16)+SUM(C10:C14)</f>
+        <v>2.5579999999999998</v>
+      </c>
+      <c r="D17" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9265000000000001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated PV default costs- CHANGES THE ANSWERS. Also added ATB reference and updated the PV default costs spreadsheet.
</commit_message>
<xml_diff>
--- a/References/PV Default Costs.xlsx
+++ b/References/PV Default Costs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
   <si>
     <t>Direct Capital Costs</t>
   </si>
@@ -88,15 +88,25 @@
   </si>
   <si>
     <t>SAM Version 2014.11.24</t>
+  </si>
+  <si>
+    <t>Engineering ($/Wdc): Changed to be "Developer Overhead ($/Wdc)"</t>
+  </si>
+  <si>
+    <t>Land preparation: Changed to be "Transmission Line ($/Wdc)"</t>
+  </si>
+  <si>
+    <t>Inverter ($/Wdc)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -130,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -176,7 +192,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -214,6 +230,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -520,7 +539,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,39 +598,53 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="16">
         <v>0.70498109471139347</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="16">
+        <v>0.69666666666666699</v>
+      </c>
       <c r="D4" s="15">
         <v>0.71</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="3">
+      <c r="E4" s="15">
+        <v>0.68</v>
+      </c>
+      <c r="F4" s="25">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="G4" s="25">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B5" s="16">
         <v>0.33219565217391261</v>
       </c>
-      <c r="C5" s="16"/>
+      <c r="C5" s="16">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="D5" s="15">
         <v>0.21</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="3">
+      <c r="E5" s="15">
+        <v>0.13</v>
+      </c>
+      <c r="F5" s="25">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="G5" s="25">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -619,65 +652,100 @@
         <f>0.606727822987794+0.21</f>
         <v>0.81672782298779401</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="16">
+        <f>0.329105205267494+0.203586501897641</f>
+        <v>0.53269170716513492</v>
+      </c>
       <c r="D6" s="15">
         <v>0.56579275109464489</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="3">
+      <c r="E6" s="15">
+        <f>0.178+0.156+0.029</f>
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="F6" s="25">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="G6" s="25">
+        <f>0.16+0.16</f>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="16">
         <v>0.3</v>
       </c>
-      <c r="C7" s="16"/>
+      <c r="C7" s="16">
+        <f>0.215199265236845+0.115106555743999</f>
+        <v>0.33030582098084399</v>
+      </c>
       <c r="D7" s="15">
         <v>0.15</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="3">
+      <c r="E7" s="15">
+        <f>0.55*0.187+0.45*0.187</f>
+        <v>0.187</v>
+      </c>
+      <c r="F7" s="25">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="G7" s="25">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="16">
         <v>0.9469103998436198</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="16">
+        <f>0.677401030654478+0.37787140321983</f>
+        <v>1.055272433874308</v>
+      </c>
       <c r="D8" s="15">
         <v>0.75</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="3">
+      <c r="E8" s="15">
+        <f>0.06+0.1661/2+0.1661/2+0.493</f>
+        <v>0.71910000000000007</v>
+      </c>
+      <c r="F8" s="25">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="G8" s="25">
+        <f>0.103724570767137+0.06</f>
+        <v>0.16372457076713698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="18">
         <v>0</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="18">
+        <v>0</v>
+      </c>
       <c r="D9" s="11">
         <v>0</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
       <c r="F9" s="12">
         <v>0</v>
       </c>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
@@ -688,35 +756,49 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="16">
         <v>9.7136303302560914E-2</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="16">
+        <v>0.11</v>
+      </c>
       <c r="D11" s="15">
         <v>5.7294635612556974E-2</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="3">
+      <c r="E11" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="F11" s="25">
         <v>0.05</v>
       </c>
+      <c r="G11" s="25">
+        <v>2.3767500513328502E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
+      <c r="A12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="25">
+        <v>0</v>
+      </c>
+      <c r="G12" s="25">
+        <f>0.16</f>
+        <v>0.16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="G13" s="25">
         <v>0.03</v>
       </c>
     </row>
@@ -724,34 +806,46 @@
       <c r="A14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="25">
         <v>0.03</v>
       </c>
+      <c r="G14" s="25">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="A15" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="25">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="G15" s="25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="10">
+        <v>0.51679868381138649</v>
+      </c>
       <c r="D16" s="11">
         <v>0.81863629229227208</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="11">
+        <v>0.67240632966186697</v>
+      </c>
       <c r="F16" s="12">
         <v>1</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -760,35 +854,50 @@
       <c r="B17" s="10">
         <v>0.05</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="10">
+        <v>0.05</v>
+      </c>
       <c r="D17" s="11">
         <v>0.05</v>
       </c>
-      <c r="E17" s="11"/>
+      <c r="E17" s="11">
+        <v>0.05</v>
+      </c>
       <c r="F17" s="12">
         <v>0.05</v>
       </c>
-      <c r="G17" s="12"/>
+      <c r="G17" s="12">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="14">
-        <f t="shared" ref="B18" si="0">SUM(B4:B8)*(1+B9)*(1+B16*B17)+SUM(B11:B15)</f>
+        <f t="shared" ref="B18:C18" si="0">SUM(B4:B8)*(1+B9)*(1+B16*B17)+SUM(B11:B15)</f>
         <v>3.2878749071410653</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="27">
+        <f>SUM(C4:C8)*(1+C9)*(1+C16*C17)+SUM(C11:C15)</f>
+        <v>3.0899999999999994</v>
+      </c>
       <c r="D18" s="14">
-        <f t="shared" ref="D18" si="1">SUM(D4:D8)*(1+D9)*(1+D16*D17)+SUM(D11:D15)</f>
+        <f t="shared" ref="D18:E18" si="1">SUM(D4:D8)*(1+D9)*(1+D16*D17)+SUM(D11:D15)</f>
         <v>2.5407422133038966</v>
       </c>
-      <c r="E18" s="14"/>
+      <c r="E18" s="14">
+        <f t="shared" si="1"/>
+        <v>2.1499999999999995</v>
+      </c>
       <c r="F18" s="14">
-        <f t="shared" ref="F18" si="2">SUM(F4:F8)*(1+F9)*(1+F16*F17)+SUM(F11:F15)</f>
+        <f t="shared" ref="F18:G18" si="2">SUM(F4:F8)*(1+F9)*(1+F16*F17)+SUM(F11:F15)</f>
         <v>1.9024999999999999</v>
       </c>
-      <c r="G18" s="14"/>
+      <c r="G18" s="14">
+        <f t="shared" si="2"/>
+        <v>1.7691782998188224</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
#releasenotes Updated PV costs for 2017.1.17 release per Ran Fu, documented in References/PV Default Costs.xlsx. Applied updates to both detailed and PVWatts models. LCOE model defaults will get updated using most recent ATB numbers.
</commit_message>
<xml_diff>
--- a/References/PV Default Costs.xlsx
+++ b/References/PV Default Costs.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="20370" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Proposed 2016.3.14" sheetId="1" r:id="rId1"/>
-    <sheet name="2014.11.24" sheetId="2" r:id="rId2"/>
-    <sheet name="2014.1.14" sheetId="3" r:id="rId3"/>
+    <sheet name="Proposed 2017.1.17" sheetId="4" r:id="rId1"/>
+    <sheet name="2016.3.14" sheetId="1" r:id="rId2"/>
+    <sheet name="2014.11.24" sheetId="2" r:id="rId3"/>
+    <sheet name="2014.1.14" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="32">
   <si>
     <t>Direct Capital Costs</t>
   </si>
@@ -97,6 +98,21 @@
   </si>
   <si>
     <t>Inverter ($/Wdc)</t>
+  </si>
+  <si>
+    <t>Battery bank (S/kWh DC)</t>
+  </si>
+  <si>
+    <t>Engineering &amp; developer overhead</t>
+  </si>
+  <si>
+    <t>Land prep. &amp; transmission</t>
+  </si>
+  <si>
+    <t>Battery Costs (NEW)</t>
+  </si>
+  <si>
+    <t>To be included in SAM Version 2017.1.17</t>
   </si>
 </sst>
 </file>
@@ -192,7 +208,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -221,18 +237,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -536,9 +553,417 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="11.28515625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="11.28515625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="28"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.64</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0.68</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0.64</v>
+      </c>
+      <c r="F4" s="22">
+        <v>0.65</v>
+      </c>
+      <c r="G4" s="22">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.21</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.13</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.13</v>
+      </c>
+      <c r="F5" s="22">
+        <v>0.11</v>
+      </c>
+      <c r="G5" s="22">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16">
+        <v>0.53</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.36</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0.36</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.33</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0.32</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0.19</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.19</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0.19</v>
+      </c>
+      <c r="G7" s="22">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="16">
+        <v>1.06</v>
+      </c>
+      <c r="C8" s="16">
+        <v>1.25</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.72</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.72</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0.16</v>
+      </c>
+      <c r="G8" s="22">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="18">
+        <v>0</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="16">
+        <v>0.11</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="22">
+        <v>0.02</v>
+      </c>
+      <c r="G11" s="22">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0.16</v>
+      </c>
+      <c r="G12" s="22">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="22">
+        <v>0.03</v>
+      </c>
+      <c r="G13" s="22">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="22">
+        <v>0.03</v>
+      </c>
+      <c r="G14" s="22">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="22">
+        <v>0.02</v>
+      </c>
+      <c r="G15" s="22">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0.52</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.52</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="F16" s="12">
+        <v>1</v>
+      </c>
+      <c r="G16" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="25">
+        <f t="shared" ref="B18:G18" si="0">SUM(B4:B8)*(1+B9)*(1+B16*B17)+SUM(B11:B15)</f>
+        <v>3.0956600000000001</v>
+      </c>
+      <c r="C18" s="25">
+        <f t="shared" si="0"/>
+        <v>2.9317600000000001</v>
+      </c>
+      <c r="D18" s="25">
+        <f t="shared" si="0"/>
+        <v>2.14968</v>
+      </c>
+      <c r="E18" s="25">
+        <f t="shared" si="0"/>
+        <v>2.127335</v>
+      </c>
+      <c r="F18" s="25">
+        <f t="shared" si="0"/>
+        <v>1.7615000000000001</v>
+      </c>
+      <c r="G18" s="25">
+        <f t="shared" si="0"/>
+        <v>1.4184999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+    </row>
+    <row r="20" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="16">
+        <v>600</v>
+      </c>
+      <c r="C21" s="16">
+        <v>500</v>
+      </c>
+      <c r="D21" s="15">
+        <v>600</v>
+      </c>
+      <c r="E21" s="15">
+        <v>500</v>
+      </c>
+      <c r="F21" s="22">
+        <v>600</v>
+      </c>
+      <c r="G21" s="22">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -554,18 +979,18 @@
       <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="22"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -614,10 +1039,10 @@
       <c r="E4" s="15">
         <v>0.68</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="22">
         <v>0.71</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="22">
         <v>0.65</v>
       </c>
     </row>
@@ -637,10 +1062,10 @@
       <c r="E5" s="15">
         <v>0.13</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="22">
         <v>0.12</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="22">
         <v>0.11</v>
       </c>
     </row>
@@ -663,10 +1088,10 @@
         <f>0.178+0.156+0.029</f>
         <v>0.36299999999999999</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <v>0.41</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="22">
         <f>0.16+0.16</f>
         <v>0.32</v>
       </c>
@@ -689,10 +1114,10 @@
         <f>0.55*0.187+0.45*0.187</f>
         <v>0.187</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="22">
         <v>0.24</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="22">
         <v>0.19</v>
       </c>
     </row>
@@ -714,10 +1139,10 @@
         <f>0.06+0.1661/2+0.1661/2+0.493</f>
         <v>0.71910000000000007</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>0.17</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="22">
         <f>0.103724570767137+0.06</f>
         <v>0.16372457076713698</v>
       </c>
@@ -772,21 +1197,21 @@
       <c r="E11" s="15">
         <v>1E-3</v>
       </c>
-      <c r="F11" s="25">
-        <v>0.05</v>
-      </c>
-      <c r="G11" s="25">
+      <c r="F11" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="G11" s="22">
         <v>2.3767500513328502E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="25">
-        <v>0</v>
-      </c>
-      <c r="G12" s="25">
+      <c r="F12" s="22">
+        <v>0</v>
+      </c>
+      <c r="G12" s="22">
         <f>0.16</f>
         <v>0.16</v>
       </c>
@@ -795,10 +1220,10 @@
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="22">
         <v>0.03</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="22">
         <v>0.03</v>
       </c>
     </row>
@@ -806,21 +1231,21 @@
       <c r="A14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="22">
         <v>0.03</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="22">
         <v>0.03</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="22">
         <v>0.06</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="22">
         <v>0.02</v>
       </c>
     </row>
@@ -875,10 +1300,10 @@
         <v>20</v>
       </c>
       <c r="B18" s="14">
-        <f t="shared" ref="B18:C18" si="0">SUM(B4:B8)*(1+B9)*(1+B16*B17)+SUM(B11:B15)</f>
+        <f t="shared" ref="B18" si="0">SUM(B4:B8)*(1+B9)*(1+B16*B17)+SUM(B11:B15)</f>
         <v>3.2878749071410653</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="24">
         <f>SUM(C4:C8)*(1+C9)*(1+C16*C17)+SUM(C11:C15)</f>
         <v>3.0899999999999994</v>
       </c>
@@ -910,7 +1335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -1137,7 +1562,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>

</xml_diff>